<commit_message>
cap nhat chuc nang xoa tren panelKhoHang
</commit_message>
<xml_diff>
--- a/Quan_Ly/Quan_Ly/bin/Debug/data/Kho Hàng.xlsx
+++ b/Quan_Ly/Quan_Ly/bin/Debug/data/Kho Hàng.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Kho Hàng</t>
   </si>
@@ -89,12 +89,6 @@
     <t>Mứt xoài</t>
   </si>
   <si>
-    <t>Mứt chanh leo</t>
-  </si>
-  <si>
-    <t>Mứt dâu</t>
-  </si>
-  <si>
     <t>Mứt kiwi</t>
   </si>
   <si>
@@ -104,19 +98,10 @@
     <t>lốc</t>
   </si>
   <si>
-    <t>Trà Lài</t>
-  </si>
-  <si>
-    <t>Ly + nắp nhựa</t>
-  </si>
-  <si>
-    <t>Ống hút</t>
-  </si>
-  <si>
     <t>Cà phê A</t>
   </si>
   <si>
-    <t>2</t>
+    <t>1</t>
   </si>
   <si>
     <t>120000</t>
@@ -171,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
@@ -203,7 +188,6 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0" applyProtection="1"/>
     <xf numFmtId="1" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -487,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
@@ -649,19 +633,19 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>1</v>
       </c>
-      <c r="D10" s="11">
-        <v>99000</v>
-      </c>
-      <c r="E10" s="11">
+      <c r="D10" s="8">
+        <v>109000</v>
+      </c>
+      <c r="E10" s="6">
         <f>C6*D6</f>
       </c>
     </row>
@@ -670,118 +654,33 @@
         <v>18</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C11" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D11" s="11">
-        <v>97000</v>
+        <v>21000</v>
       </c>
       <c r="E11" s="11">
         <f>C6*D6</f>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="5">
-        <v>1</v>
-      </c>
-      <c r="D12" s="11">
-        <v>109000</v>
-      </c>
-      <c r="E12" s="11">
-        <f>C6*D6</f>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="10" t="s">
+      <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="5">
-        <v>6</v>
-      </c>
-      <c r="D13" s="11">
-        <v>21000</v>
-      </c>
-      <c r="E13" s="11">
-        <f>C6*D6</f>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="10" t="s">
+      <c r="D12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="5">
-        <v>1</v>
-      </c>
-      <c r="D14" s="11">
-        <v>255000</v>
-      </c>
-      <c r="E14" s="11">
-        <f>C6*D6</f>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="5">
-        <v>50</v>
-      </c>
-      <c r="D15" s="11">
-        <v>48000</v>
-      </c>
-      <c r="E15" s="11">
-        <f>C6*D6</f>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="5">
-        <v>2</v>
-      </c>
-      <c r="D16" s="11">
-        <v>18000</v>
-      </c>
-      <c r="E16" s="11">
-        <f>C6*D6</f>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="6">
-        <f>C17*D17</f>
+      <c r="E12" s="6">
+        <f>C12*D12</f>
       </c>
     </row>
   </sheetData>

</xml_diff>